<commit_message>
Auto-committed on 2022/08/23 週二 16:25:11.81
</commit_message>
<xml_diff>
--- a/Program/Other/L5915_底稿_協辦人員業績統計_件數及金額明細.xlsx
+++ b/Program/Other/L5915_底稿_協辦人員業績統計_件數及金額明細.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA494648-748C-40CD-9115-5CE1BB745823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0925DDA9-86F4-4D23-806A-6808B72CA28B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="791" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="791" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="件數" sheetId="70" r:id="rId1"/>
@@ -75,58 +75,70 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
+  <si>
+    <t>戶號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>員工姓名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>部室</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>區部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>單位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>員工代號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>獎金類別</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>戶號</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>計件代碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>撥款金額</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>戶名</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>車馬費發放額</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>介紹人</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>員工姓名</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>部室</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>區部</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>單位</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>員工代號</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>額度</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>撥款金額</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>計件代碼</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>統一編號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>額度號碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>已用額度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>發放日期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>發放金額</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>額度編號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -136,13 +148,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5">
-    <font>
-      <sz val="12"/>
-      <name val="新細明體"/>
-      <family val="1"/>
-      <charset val="136"/>
-    </font>
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <name val="新細明體"/>
@@ -170,18 +176,12 @@
       <charset val="136"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -197,22 +197,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -606,57 +609,67 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0869A94A-3298-4599-A82F-79706276E934}">
   <sheetPr codeName="工作表1"/>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="18.6640625" style="2"/>
+    <col min="1" max="15" width="10.77734375" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="18.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -666,54 +679,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F5A011B-B6C8-45CD-9219-0AEAA3A08C8A}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="16.2"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="6" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" style="2" customWidth="1"/>
-    <col min="4" max="5" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="15.77734375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="18.6640625" style="2"/>
+    <col min="1" max="3" width="10.77734375" style="1"/>
+    <col min="4" max="4" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
+      <c r="G1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>